<commit_message>
Agrego "Genere el reporte de las métricas del proyecto"
</commit_message>
<xml_diff>
--- a/2da parte/Composicion de algoritmos/Especificaciones/Muestre las métricas de un proyecto.xlsx
+++ b/2da parte/Composicion de algoritmos/Especificaciones/Muestre las métricas de un proyecto.xlsx
@@ -9,14 +9,15 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20220" windowHeight="8925" firstSheet="2" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20220" windowHeight="8925" firstSheet="2" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Introducción" sheetId="6" state="hidden" r:id="rId1"/>
     <sheet name="Cómo programarlo" sheetId="7" state="hidden" r:id="rId2"/>
-    <sheet name="escalar" sheetId="1" r:id="rId3"/>
-    <sheet name="estructura de datos" sheetId="4" r:id="rId4"/>
-    <sheet name="lista de estructuras de datos" sheetId="5" r:id="rId5"/>
+    <sheet name="reporte de metricas" sheetId="8" r:id="rId3"/>
+    <sheet name="lista de metricas" sheetId="5" r:id="rId4"/>
+    <sheet name="metricas de una iteracion" sheetId="4" r:id="rId5"/>
+    <sheet name="calculos" sheetId="1" r:id="rId6"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -51,6 +52,104 @@
 </file>
 
 <file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Centeno, Oscar</author>
+  </authors>
+  <commentList>
+    <comment ref="I8" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Asuma que la capacidad del equipo nunca será cero.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C20" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">La suma de todos los puntos de las historias que fueron introducidas en la iteracion actual o en las anteriores, y se le resta los puntos de las historas que fueron sacadas del alcance en la iteración actual o en las anteriores.
+</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments3.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Centeno, Oscar</author>
+  </authors>
+  <commentList>
+    <comment ref="I4" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Asuma que la capacidad del equipo nunca será cero.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C11" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">La suma de todos los puntos de las historias que fueron introducidas en la iteracion actual o en las anteriores, y se le resta los puntos de las historas que fueron sacadas del alcance en la iteración actual o en las anteriores.
+</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments4.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Centeno, Oscar</author>
+  </authors>
+  <commentList>
+    <comment ref="C9" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">La suma de todos los puntos de las historias que fueron introducidas en la iteracion actual o en las anteriores, y se le resta los puntos de las historas que fueron sacadas del alcance en la iteración actual o en las anteriores.
+</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments5.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>Centeno, Oscar</author>
@@ -99,69 +198,8 @@
 </comments>
 </file>
 
-<file path=xl/comments3.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <authors>
-    <author>Centeno, Oscar</author>
-  </authors>
-  <commentList>
-    <comment ref="C9" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">La suma de todos los puntos de las historias que fueron introducidas en la iteracion actual o en las anteriores, y se le resta los puntos de las historas que fueron sacadas del alcance en la iteración actual o en las anteriores.
-</t>
-        </r>
-      </text>
-    </comment>
-  </commentList>
-</comments>
-</file>
-
-<file path=xl/comments4.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <authors>
-    <author>Centeno, Oscar</author>
-  </authors>
-  <commentList>
-    <comment ref="I6" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t>Asuma que la capacidad del equipo nunca será cero.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="C13" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">La suma de todos los puntos de las historias que fueron introducidas en la iteracion actual o en las anteriores, y se le resta los puntos de las historas que fueron sacadas del alcance en la iteración actual o en las anteriores.
-</t>
-        </r>
-      </text>
-    </comment>
-  </commentList>
-</comments>
-</file>
-
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="150">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="261" uniqueCount="159">
   <si>
     <t>Genere la métrica de puntos</t>
   </si>
@@ -514,9 +552,6 @@
     <t>fecha final</t>
   </si>
   <si>
-    <t>Algoritmos que retornan listas de estructuras de datos</t>
-  </si>
-  <si>
     <t>las iteraciones del proyecto</t>
   </si>
   <si>
@@ -611,6 +646,36 @@
   </si>
   <si>
     <t>Además, siempre utilice las palabras del negocio, no palabras técnicas o abreviaturas que no sean comunes.</t>
+  </si>
+  <si>
+    <t>Genere el reporte de las métricas del proyecto</t>
+  </si>
+  <si>
+    <t>Dado</t>
+  </si>
+  <si>
+    <t>Y</t>
+  </si>
+  <si>
+    <t>sus iteraciones</t>
+  </si>
+  <si>
+    <t>Nombre</t>
+  </si>
+  <si>
+    <t>Proyecto asombroso</t>
+  </si>
+  <si>
+    <t>el reporte indica</t>
+  </si>
+  <si>
+    <t>las métricas de cada iteración</t>
+  </si>
+  <si>
+    <t>el proyecto</t>
+  </si>
+  <si>
+    <t>se consulta el reporte del proyecto</t>
   </si>
 </sst>
 </file>
@@ -741,7 +806,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="8">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -824,6 +889,21 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="4"/>
+      </left>
+      <right style="thin">
+        <color theme="4"/>
+      </right>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="thin">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -837,7 +917,7 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -879,6 +959,11 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="10">
     <cellStyle name="20% - Accent1" xfId="6" builtinId="30"/>
@@ -892,7 +977,7 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="9" builtinId="5"/>
   </cellStyles>
-  <dxfs count="38">
+  <dxfs count="53">
     <dxf>
       <font>
         <b val="0"/>
@@ -909,37 +994,50 @@
         <name val="Calibri"/>
         <scheme val="minor"/>
       </font>
-      <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
       <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right style="thin">
-          <color theme="4"/>
-        </right>
+        <left style="thin">
+          <color theme="4"/>
+        </left>
+        <right/>
         <top style="thin">
           <color theme="4"/>
         </top>
-        <bottom style="thin">
-          <color theme="4"/>
-        </bottom>
+        <bottom/>
         <vertical/>
         <horizontal/>
       </border>
     </dxf>
     <dxf>
-      <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
-      <border diagonalUp="0" diagonalDown="0">
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="0"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4"/>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <border outline="0">
         <left style="thin">
           <color theme="4"/>
         </left>
-        <right/>
         <top style="thin">
           <color theme="4"/>
         </top>
-        <bottom style="thin">
-          <color theme="4"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
       </border>
     </dxf>
     <dxf>
@@ -958,13 +1056,35 @@
         <name val="Calibri"/>
         <scheme val="minor"/>
       </font>
+      <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
       <border diagonalUp="0" diagonalDown="0">
         <left/>
+        <right style="thin">
+          <color theme="4"/>
+        </right>
+        <top style="thin">
+          <color theme="4"/>
+        </top>
+        <bottom style="thin">
+          <color theme="4"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color theme="4"/>
+        </left>
         <right/>
         <top style="thin">
           <color theme="4"/>
         </top>
-        <bottom/>
+        <bottom style="thin">
+          <color theme="4"/>
+        </bottom>
         <vertical/>
         <horizontal/>
       </border>
@@ -1093,7 +1213,6 @@
         <name val="Calibri"/>
         <scheme val="minor"/>
       </font>
-      <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
       <border diagonalUp="0" diagonalDown="0">
         <left/>
         <right/>
@@ -1124,9 +1243,7 @@
       <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
       <border diagonalUp="0" diagonalDown="0">
         <left/>
-        <right style="thin">
-          <color theme="4"/>
-        </right>
+        <right/>
         <top style="thin">
           <color theme="4"/>
         </top>
@@ -1153,10 +1270,10 @@
       </font>
       <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
       <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color theme="4"/>
-        </left>
-        <right/>
+        <left/>
+        <right style="thin">
+          <color theme="4"/>
+        </right>
         <top style="thin">
           <color theme="4"/>
         </top>
@@ -1181,6 +1298,36 @@
         <name val="Calibri"/>
         <scheme val="minor"/>
       </font>
+      <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color theme="4"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color theme="4"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <scheme val="none"/>
+      </font>
     </dxf>
     <dxf>
       <font>
@@ -1221,13 +1368,35 @@
         <name val="Calibri"/>
         <scheme val="minor"/>
       </font>
+      <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
       <border diagonalUp="0" diagonalDown="0">
         <left/>
+        <right style="thin">
+          <color theme="4"/>
+        </right>
+        <top style="thin">
+          <color theme="4"/>
+        </top>
+        <bottom style="thin">
+          <color theme="4"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color theme="4"/>
+        </left>
         <right/>
         <top style="thin">
           <color theme="4"/>
         </top>
-        <bottom/>
+        <bottom style="thin">
+          <color theme="4"/>
+        </bottom>
         <vertical/>
         <horizontal/>
       </border>
@@ -1356,7 +1525,6 @@
         <name val="Calibri"/>
         <scheme val="minor"/>
       </font>
-      <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
       <border diagonalUp="0" diagonalDown="0">
         <left/>
         <right/>
@@ -1387,9 +1555,7 @@
       <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
       <border diagonalUp="0" diagonalDown="0">
         <left/>
-        <right style="thin">
-          <color theme="4"/>
-        </right>
+        <right/>
         <top style="thin">
           <color theme="4"/>
         </top>
@@ -1415,13 +1581,17 @@
         <scheme val="minor"/>
       </font>
       <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
+      <border diagonalUp="0" diagonalDown="0">
         <left/>
-        <right/>
+        <right style="thin">
+          <color theme="4"/>
+        </right>
         <top style="thin">
           <color theme="4"/>
         </top>
         <bottom/>
+        <vertical/>
+        <horizontal/>
       </border>
     </dxf>
     <dxf>
@@ -1440,26 +1610,18 @@
         <name val="Calibri"/>
         <scheme val="minor"/>
       </font>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
+      <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color theme="4"/>
+        </left>
         <right/>
         <top style="thin">
           <color theme="4"/>
         </top>
         <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <left style="thin">
-          <color theme="4"/>
-        </left>
-        <right style="thin">
-          <color theme="4"/>
-        </right>
-        <top style="thin">
-          <color theme="4"/>
-        </top>
+        <vertical/>
+        <horizontal/>
       </border>
     </dxf>
     <dxf>
@@ -1518,26 +1680,8 @@
         <name val="Calibri"/>
         <scheme val="minor"/>
       </font>
-      <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
       <border diagonalUp="0" diagonalDown="0">
         <left/>
-        <right style="thin">
-          <color theme="4"/>
-        </right>
-        <top style="thin">
-          <color theme="4"/>
-        </top>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color theme="4"/>
-        </left>
         <right/>
         <top style="thin">
           <color theme="4"/>
@@ -1563,16 +1707,16 @@
         <name val="Calibri"/>
         <scheme val="minor"/>
       </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
     </dxf>
     <dxf>
       <font>
@@ -1617,6 +1761,321 @@
         <name val="Calibri"/>
         <scheme val="minor"/>
       </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thin">
+          <color theme="4"/>
+        </right>
+        <top style="thin">
+          <color theme="4"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <left style="thin">
+          <color theme="4"/>
+        </left>
+        <right style="thin">
+          <color theme="4"/>
+        </right>
+        <top style="thin">
+          <color theme="4"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="0"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4"/>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thin">
+          <color theme="4"/>
+        </right>
+        <top style="thin">
+          <color theme="4"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color theme="4"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color theme="4"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
       <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
       <border diagonalUp="0" diagonalDown="0">
         <left/>
@@ -1737,8 +2196,8 @@
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
     <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
-      <tableStyleElement type="wholeTable" dxfId="37"/>
-      <tableStyleElement type="headerRow" dxfId="36"/>
+      <tableStyleElement type="wholeTable" dxfId="52"/>
+      <tableStyleElement type="headerRow" dxfId="51"/>
     </tableStyle>
   </tableStyles>
   <extLst>
@@ -1765,34 +2224,29 @@
 </table>
 </file>
 
-<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="16" name="Table17" displayName="Table17" ref="C57:D64" totalsRowShown="0">
-  <autoFilter ref="C57:D64"/>
-  <tableColumns count="2">
-    <tableColumn id="1" name="Historia terminada en iteración" dataDxfId="35"/>
-    <tableColumn id="2" name="Puntos de la historia" dataDxfId="34"/>
+<file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="22" name="Table22" displayName="Table22" ref="B5:J6" totalsRowShown="0" headerRowDxfId="38" dataDxfId="37" tableBorderDxfId="36">
+  <autoFilter ref="B5:J6"/>
+  <tableColumns count="9">
+    <tableColumn id="1" name="Numero" dataDxfId="35"/>
+    <tableColumn id="2" name="Fecha inicial" dataDxfId="34"/>
+    <tableColumn id="3" name="Fecha final" dataDxfId="33"/>
+    <tableColumn id="10" name="Hay informacion de puntos disponible" dataDxfId="32"/>
+    <tableColumn id="4" name="Puntos planificados" dataDxfId="31"/>
+    <tableColumn id="5" name="Puntos terminados" dataDxfId="30"/>
+    <tableColumn id="6" name="Hay informacion de dias disponible" dataDxfId="29"/>
+    <tableColumn id="7" name="Capacidad del equipo" dataDxfId="28"/>
+    <tableColumn id="8" name="Dias no efectivos" dataDxfId="27"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
-<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="17" name="Table1118" displayName="Table1118" ref="B69:D72" totalsRowShown="0" headerRowDxfId="33" tableBorderDxfId="32">
-  <autoFilter ref="B69:D72"/>
-  <tableColumns count="3">
-    <tableColumn id="1" name="Ejemplo" dataDxfId="31"/>
-    <tableColumn id="2" name="Iteración" dataDxfId="30"/>
-    <tableColumn id="3" name="Velocidad" dataDxfId="29"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table11.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="B9:F14" totalsRowShown="0">
   <autoFilter ref="B9:F14"/>
   <tableColumns count="5">
-    <tableColumn id="1" name="Ejemplo" dataDxfId="28"/>
+    <tableColumn id="1" name="Ejemplo" dataDxfId="43"/>
     <tableColumn id="2" name="Puntos planificados"/>
     <tableColumn id="3" name="Puntos terminados"/>
     <tableColumn id="4" name="Hay informacion de puntos disponible"/>
@@ -1802,12 +2256,12 @@
 </table>
 </file>
 
-<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table12.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table14" displayName="Table14" ref="B25:F29" totalsRowShown="0">
   <autoFilter ref="B25:F29"/>
   <tableColumns count="5">
-    <tableColumn id="1" name="Ejemplo" dataDxfId="27"/>
-    <tableColumn id="6" name="Hay informacion de dias disponible" dataDxfId="26"/>
+    <tableColumn id="1" name="Ejemplo" dataDxfId="42"/>
+    <tableColumn id="6" name="Hay informacion de dias disponible" dataDxfId="41"/>
     <tableColumn id="2" name="Capacidad del equipo"/>
     <tableColumn id="3" name="Dias no efectivos"/>
     <tableColumn id="5" name="Tiempo no efectivo"/>
@@ -1816,67 +2270,114 @@
 </table>
 </file>
 
-<file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="19" name="Table412" displayName="Table412" ref="B9:F10" totalsRowShown="0">
-  <autoFilter ref="B9:F10"/>
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="16" name="Table17" displayName="Table17" ref="C57:D64" totalsRowShown="0">
+  <autoFilter ref="C57:D64"/>
+  <tableColumns count="2">
+    <tableColumn id="1" name="Historia terminada en iteración" dataDxfId="50"/>
+    <tableColumn id="2" name="Puntos de la historia" dataDxfId="49"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="17" name="Table1118" displayName="Table1118" ref="B69:D72" totalsRowShown="0" headerRowDxfId="48" tableBorderDxfId="47">
+  <autoFilter ref="B69:D72"/>
+  <tableColumns count="3">
+    <tableColumn id="1" name="Ejemplo" dataDxfId="46"/>
+    <tableColumn id="2" name="Iteración" dataDxfId="45"/>
+    <tableColumn id="3" name="Velocidad" dataDxfId="44"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table18193" displayName="Table18193" ref="B8:J11" totalsRowShown="0" headerRowDxfId="14" dataDxfId="13">
+  <autoFilter ref="B8:J11"/>
+  <tableColumns count="9">
+    <tableColumn id="1" name="Numero"/>
+    <tableColumn id="2" name="fecha inicial" dataDxfId="12"/>
+    <tableColumn id="3" name="fecha final" dataDxfId="11"/>
+    <tableColumn id="10" name="Hay informacion de puntos disponible" dataDxfId="10"/>
+    <tableColumn id="4" name="Puntos planificados" dataDxfId="9"/>
+    <tableColumn id="5" name="Puntos terminados" dataDxfId="8"/>
+    <tableColumn id="6" name="Hay informacion de dias disponible" dataDxfId="7"/>
+    <tableColumn id="7" name="Capacidad del equipo" dataDxfId="6"/>
+    <tableColumn id="8" name="Dias no efectivos" dataDxfId="5"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table412245" displayName="Table412245" ref="B20:F23" totalsRowShown="0">
+  <autoFilter ref="B20:F23"/>
   <tableColumns count="5">
     <tableColumn id="1" name="Iteración"/>
-    <tableColumn id="2" name="Fecha inicial" dataDxfId="25"/>
-    <tableColumn id="6" name="Fecha final" dataDxfId="24"/>
+    <tableColumn id="2" name="Fecha inicial" dataDxfId="4"/>
+    <tableColumn id="6" name="Fecha final" dataDxfId="3"/>
     <tableColumn id="4" name="Métrica de puntos"/>
     <tableColumn id="5" name="Métrica de tiempo no efectivo"/>
   </tableColumns>
-  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+  <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table5" displayName="Table5" ref="B4:B5" totalsRowShown="0" headerRowDxfId="1" tableBorderDxfId="2">
+  <autoFilter ref="B4:B5"/>
+  <tableColumns count="1">
+    <tableColumn id="1" name="Nombre" dataDxfId="0"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="22" name="Table22" displayName="Table22" ref="B5:J6" totalsRowShown="0" headerRowDxfId="23" dataDxfId="22" tableBorderDxfId="21">
-  <autoFilter ref="B5:J6"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="18" name="Table1819" displayName="Table1819" ref="B4:J7" totalsRowShown="0" headerRowDxfId="26" dataDxfId="25">
+  <autoFilter ref="B4:J7"/>
   <tableColumns count="9">
-    <tableColumn id="1" name="Numero" dataDxfId="20"/>
-    <tableColumn id="2" name="Fecha inicial" dataDxfId="19"/>
-    <tableColumn id="3" name="Fecha final" dataDxfId="18"/>
-    <tableColumn id="10" name="Hay informacion de puntos disponible" dataDxfId="17"/>
-    <tableColumn id="4" name="Puntos planificados" dataDxfId="16"/>
-    <tableColumn id="5" name="Puntos terminados" dataDxfId="15"/>
-    <tableColumn id="6" name="Hay informacion de dias disponible" dataDxfId="14"/>
-    <tableColumn id="7" name="Capacidad del equipo" dataDxfId="13"/>
-    <tableColumn id="8" name="Dias no efectivos" dataDxfId="12"/>
+    <tableColumn id="1" name="Numero"/>
+    <tableColumn id="2" name="fecha inicial" dataDxfId="24"/>
+    <tableColumn id="3" name="fecha final" dataDxfId="23"/>
+    <tableColumn id="10" name="Hay informacion de puntos disponible" dataDxfId="22"/>
+    <tableColumn id="4" name="Puntos planificados" dataDxfId="21"/>
+    <tableColumn id="5" name="Puntos terminados" dataDxfId="20"/>
+    <tableColumn id="6" name="Hay informacion de dias disponible" dataDxfId="19"/>
+    <tableColumn id="7" name="Capacidad del equipo" dataDxfId="18"/>
+    <tableColumn id="8" name="Dias no efectivos" dataDxfId="17"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="18" name="Table1819" displayName="Table1819" ref="B6:J9" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
-  <autoFilter ref="B6:J9"/>
-  <tableColumns count="9">
-    <tableColumn id="1" name="Numero"/>
-    <tableColumn id="2" name="fecha inicial" dataDxfId="9"/>
-    <tableColumn id="3" name="fecha final" dataDxfId="8"/>
-    <tableColumn id="10" name="Hay informacion de puntos disponible" dataDxfId="7"/>
-    <tableColumn id="4" name="Puntos planificados" dataDxfId="6"/>
-    <tableColumn id="5" name="Puntos terminados" dataDxfId="5"/>
-    <tableColumn id="6" name="Hay informacion de dias disponible" dataDxfId="4"/>
-    <tableColumn id="7" name="Capacidad del equipo" dataDxfId="3"/>
-    <tableColumn id="8" name="Dias no efectivos" dataDxfId="2"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="23" name="Table41224" displayName="Table41224" ref="B11:F14" totalsRowShown="0">
+  <autoFilter ref="B11:F14"/>
+  <tableColumns count="5">
+    <tableColumn id="1" name="Iteración"/>
+    <tableColumn id="2" name="Fecha inicial" dataDxfId="16"/>
+    <tableColumn id="6" name="Fecha final" dataDxfId="15"/>
+    <tableColumn id="4" name="Métrica de puntos"/>
+    <tableColumn id="5" name="Métrica de tiempo no efectivo"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="23" name="Table41224" displayName="Table41224" ref="B13:F16" totalsRowShown="0">
-  <autoFilter ref="B13:F16"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="19" name="Table412" displayName="Table412" ref="B9:F10" totalsRowShown="0">
+  <autoFilter ref="B9:F10"/>
   <tableColumns count="5">
     <tableColumn id="1" name="Iteración"/>
-    <tableColumn id="2" name="Fecha inicial" dataDxfId="1"/>
-    <tableColumn id="6" name="Fecha final" dataDxfId="0"/>
+    <tableColumn id="2" name="Fecha inicial" dataDxfId="40"/>
+    <tableColumn id="6" name="Fecha final" dataDxfId="39"/>
     <tableColumn id="4" name="Métrica de puntos"/>
     <tableColumn id="5" name="Métrica de tiempo no efectivo"/>
   </tableColumns>
-  <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
@@ -2366,7 +2867,7 @@
         <v>1</v>
       </c>
       <c r="C34" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
@@ -2385,7 +2886,7 @@
         <v>72</v>
       </c>
       <c r="E38" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
@@ -2454,7 +2955,7 @@
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B45" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="47" spans="1:5" ht="18" thickBot="1" x14ac:dyDescent="0.35">
@@ -2674,139 +3175,139 @@
     <row r="83" spans="1:1" s="19" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="84" spans="1:1" s="19" customFormat="1" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A84" s="30" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="85" spans="1:1" s="19" customFormat="1" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A85" s="25" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="86" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="87" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="89" spans="1:1" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A89" s="7" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="90" spans="1:1" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
     <row r="91" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A91" s="2" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="92" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="93" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="94" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="95" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="96" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A96" s="19" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="98" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A98" s="2" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="99" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="100" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A100" s="19" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="101" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A101" s="19" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="102" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A102" s="19" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="104" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A104" s="2" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="105" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="106" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="107" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="108" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="112" spans="1:1" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A112" s="7" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="113" spans="1:1" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
     <row r="114" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A114" s="5" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="115" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="116" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="117" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="118" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
   </sheetData>
@@ -2940,315 +3441,570 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F31"/>
+  <dimension ref="A1:J23"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.7109375" customWidth="1"/>
-    <col min="2" max="2" width="36.5703125" customWidth="1"/>
-    <col min="3" max="3" width="22" customWidth="1"/>
-    <col min="4" max="4" width="20.85546875" customWidth="1"/>
-    <col min="5" max="5" width="21.28515625" customWidth="1"/>
-    <col min="6" max="6" width="13.5703125" customWidth="1"/>
-    <col min="7" max="7" width="33.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.42578125" style="32" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.5703125" style="32" customWidth="1"/>
+    <col min="3" max="3" width="19.28515625" style="32" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.85546875" style="32" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="37.7109375" style="32" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="30.7109375" style="32" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="20.28515625" style="32" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="35" style="32" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="22.5703125" style="32" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="18.42578125" style="32" bestFit="1" customWidth="1"/>
+    <col min="11" max="16384" width="9.140625" style="32"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>92</v>
       </c>
-      <c r="B1" s="32" t="s">
+      <c r="B1" s="33" t="s">
+        <v>149</v>
+      </c>
+      <c r="C1" s="33"/>
+      <c r="D1" s="33"/>
+      <c r="E1" s="33"/>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="B3" s="32" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" s="2"/>
+      <c r="B4" s="8" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5" s="2"/>
+      <c r="B5" s="35" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6" s="2"/>
+      <c r="B6" s="11"/>
+      <c r="C6" s="27"/>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="B7" s="32" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B8" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C8" s="32" t="s">
+        <v>115</v>
+      </c>
+      <c r="D8" s="32" t="s">
+        <v>116</v>
+      </c>
+      <c r="E8" s="20" t="s">
+        <v>9</v>
+      </c>
+      <c r="F8" s="20" t="s">
+        <v>7</v>
+      </c>
+      <c r="G8" s="20" t="s">
+        <v>8</v>
+      </c>
+      <c r="H8" s="20" t="s">
+        <v>26</v>
+      </c>
+      <c r="I8" s="20" t="s">
+        <v>24</v>
+      </c>
+      <c r="J8" s="20" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B9" s="5">
+        <v>1</v>
+      </c>
+      <c r="C9" s="21">
+        <v>43024</v>
+      </c>
+      <c r="D9" s="22">
+        <v>43028</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="F9" s="4">
+        <v>10</v>
+      </c>
+      <c r="G9" s="4">
+        <v>8</v>
+      </c>
+      <c r="H9" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="I9" s="4">
+        <v>100</v>
+      </c>
+      <c r="J9" s="4">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B10" s="32">
+        <v>2</v>
+      </c>
+      <c r="C10" s="23">
+        <v>43031</v>
+      </c>
+      <c r="D10" s="24">
+        <v>43035</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="F10" s="4">
         <v>0</v>
       </c>
-      <c r="C1" s="32"/>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" s="19" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
+      <c r="G10" s="4">
+        <v>0</v>
+      </c>
+      <c r="H10" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="I10" s="4">
+        <v>35</v>
+      </c>
+      <c r="J10" s="4">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B11" s="32">
+        <v>3</v>
+      </c>
+      <c r="C11" s="21">
+        <v>43038</v>
+      </c>
+      <c r="D11" s="22">
+        <v>43042</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="F11" s="4">
+        <v>0</v>
+      </c>
+      <c r="G11" s="4">
+        <v>0</v>
+      </c>
+      <c r="H11" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="I11" s="4">
+        <v>0</v>
+      </c>
+      <c r="J11" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B5" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
+      <c r="B13" s="32" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A14" s="2"/>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B6" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="B9" t="s">
-        <v>6</v>
-      </c>
-      <c r="C9" t="s">
-        <v>7</v>
-      </c>
-      <c r="D9" t="s">
-        <v>8</v>
-      </c>
-      <c r="E9" s="31" t="s">
-        <v>9</v>
-      </c>
-      <c r="F9" s="31" t="s">
+      <c r="B15" s="32" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B16" s="34" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B17" s="36" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="B19" s="37" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B20" s="32" t="s">
+        <v>40</v>
+      </c>
+      <c r="C20" s="32" t="s">
+        <v>30</v>
+      </c>
+      <c r="D20" s="32" t="s">
+        <v>31</v>
+      </c>
+      <c r="E20" s="32" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B10" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="C10">
-        <v>100</v>
-      </c>
-      <c r="D10">
-        <v>95</v>
-      </c>
-      <c r="E10" t="s">
-        <v>12</v>
-      </c>
-      <c r="F10" s="1">
-        <v>0.95</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B11" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="C11">
-        <v>99</v>
-      </c>
-      <c r="D11">
-        <v>90</v>
-      </c>
-      <c r="E11" t="s">
-        <v>12</v>
-      </c>
-      <c r="F11" s="1">
-        <v>0.91</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B12" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="C12">
-        <v>9.5</v>
-      </c>
-      <c r="D12">
-        <v>8.5</v>
-      </c>
-      <c r="E12" t="s">
-        <v>12</v>
-      </c>
-      <c r="F12" s="1">
-        <v>0.89</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B13" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="C13">
-        <v>0</v>
-      </c>
-      <c r="D13">
-        <v>10</v>
-      </c>
-      <c r="E13" t="s">
-        <v>12</v>
-      </c>
-      <c r="F13" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B14" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="C14">
-        <v>0</v>
-      </c>
-      <c r="D14">
-        <v>0</v>
-      </c>
-      <c r="E14" t="s">
-        <v>13</v>
-      </c>
-      <c r="F14" t="s">
+      <c r="F20" s="32" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B21" s="32">
+        <v>1</v>
+      </c>
+      <c r="C21" s="21">
+        <v>43024</v>
+      </c>
+      <c r="D21" s="22">
+        <v>43028</v>
+      </c>
+      <c r="E21" s="1">
+        <v>0.8</v>
+      </c>
+      <c r="F21" s="1">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B22" s="32">
+        <v>2</v>
+      </c>
+      <c r="C22" s="23">
+        <v>43031</v>
+      </c>
+      <c r="D22" s="24">
+        <v>43035</v>
+      </c>
+      <c r="E22" s="32" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" s="6" t="s">
-        <v>92</v>
-      </c>
-      <c r="B17" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" s="3" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" s="19" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="3" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B21" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A22" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B22" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A24" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B25" t="s">
-        <v>6</v>
-      </c>
-      <c r="C25" t="s">
-        <v>26</v>
-      </c>
-      <c r="D25" t="s">
-        <v>24</v>
-      </c>
-      <c r="E25" t="s">
-        <v>25</v>
-      </c>
-      <c r="F25" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B26" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="C26" t="s">
-        <v>12</v>
-      </c>
-      <c r="D26">
-        <v>100</v>
-      </c>
-      <c r="E26">
-        <v>5</v>
-      </c>
-      <c r="F26" s="1">
-        <v>0.05</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B27" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="C27" t="s">
-        <v>12</v>
-      </c>
-      <c r="D27">
-        <v>99</v>
-      </c>
-      <c r="E27">
-        <v>5.67</v>
-      </c>
-      <c r="F27" s="1">
-        <v>5.7000000000000002E-2</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B28" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="C28" t="s">
-        <v>12</v>
-      </c>
-      <c r="D28">
-        <v>100</v>
-      </c>
-      <c r="E28">
-        <v>0</v>
-      </c>
-      <c r="F28" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B29" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="C29" t="s">
-        <v>13</v>
-      </c>
-      <c r="D29">
-        <v>0</v>
-      </c>
-      <c r="E29">
-        <v>0</v>
-      </c>
-      <c r="F29" t="s">
+      <c r="F22" s="29">
+        <f>10/35</f>
+        <v>0.2857142857142857</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B23" s="32">
+        <v>3</v>
+      </c>
+      <c r="C23" s="21">
+        <v>43038</v>
+      </c>
+      <c r="D23" s="22">
+        <v>43042</v>
+      </c>
+      <c r="E23" s="32" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A30" s="5"/>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="E31" s="19"/>
+      <c r="F23" s="32" t="s">
+        <v>16</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="B1:E1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>
-  <tableParts count="2">
+  <tableParts count="3">
     <tablePart r:id="rId3"/>
     <tablePart r:id="rId4"/>
+    <tablePart r:id="rId5"/>
   </tableParts>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J14"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:E1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="14.42578125" customWidth="1"/>
+    <col min="2" max="2" width="26.140625" customWidth="1"/>
+    <col min="3" max="3" width="37.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.140625" customWidth="1"/>
+    <col min="5" max="5" width="37.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="34.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="30.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="35" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="22.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="18.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="B1" s="33" t="s">
+        <v>143</v>
+      </c>
+      <c r="C1" s="33"/>
+      <c r="D1" s="33"/>
+      <c r="E1" s="33"/>
+    </row>
+    <row r="3" spans="1:10" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B3" s="19" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C4" s="19" t="s">
+        <v>115</v>
+      </c>
+      <c r="D4" s="19" t="s">
+        <v>116</v>
+      </c>
+      <c r="E4" s="20" t="s">
+        <v>9</v>
+      </c>
+      <c r="F4" s="20" t="s">
+        <v>7</v>
+      </c>
+      <c r="G4" s="20" t="s">
+        <v>8</v>
+      </c>
+      <c r="H4" s="20" t="s">
+        <v>26</v>
+      </c>
+      <c r="I4" s="20" t="s">
+        <v>24</v>
+      </c>
+      <c r="J4" s="20" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="5">
+        <v>1</v>
+      </c>
+      <c r="C5" s="21">
+        <v>43024</v>
+      </c>
+      <c r="D5" s="22">
+        <v>43028</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="F5" s="4">
+        <v>10</v>
+      </c>
+      <c r="G5" s="4">
+        <v>8</v>
+      </c>
+      <c r="H5" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="I5" s="4">
+        <v>100</v>
+      </c>
+      <c r="J5" s="4">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="19">
+        <v>2</v>
+      </c>
+      <c r="C6" s="23">
+        <v>43031</v>
+      </c>
+      <c r="D6" s="24">
+        <v>43035</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="F6" s="4">
+        <v>0</v>
+      </c>
+      <c r="G6" s="4">
+        <v>0</v>
+      </c>
+      <c r="H6" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="I6" s="4">
+        <v>35</v>
+      </c>
+      <c r="J6" s="4">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B7" s="19">
+        <v>3</v>
+      </c>
+      <c r="C7" s="21">
+        <v>43038</v>
+      </c>
+      <c r="D7" s="22">
+        <v>43042</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="F7" s="4">
+        <v>0</v>
+      </c>
+      <c r="G7" s="4">
+        <v>0</v>
+      </c>
+      <c r="H7" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="I7" s="4">
+        <v>0</v>
+      </c>
+      <c r="J7" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" s="19" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="9" spans="1:10" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B9" s="19" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B10" s="19" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="19" t="s">
+        <v>40</v>
+      </c>
+      <c r="C11" s="19" t="s">
+        <v>30</v>
+      </c>
+      <c r="D11" s="19" t="s">
+        <v>31</v>
+      </c>
+      <c r="E11" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="F11" s="19" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B12" s="19">
+        <v>1</v>
+      </c>
+      <c r="C12" s="21">
+        <v>43024</v>
+      </c>
+      <c r="D12" s="22">
+        <v>43028</v>
+      </c>
+      <c r="E12" s="1">
+        <v>0.8</v>
+      </c>
+      <c r="F12" s="1">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B13" s="19">
+        <v>2</v>
+      </c>
+      <c r="C13" s="23">
+        <v>43031</v>
+      </c>
+      <c r="D13" s="24">
+        <v>43035</v>
+      </c>
+      <c r="E13" s="19" t="s">
+        <v>16</v>
+      </c>
+      <c r="F13" s="29">
+        <f>10/35</f>
+        <v>0.2857142857142857</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B14">
+        <v>3</v>
+      </c>
+      <c r="C14" s="21">
+        <v>43038</v>
+      </c>
+      <c r="D14" s="22">
+        <v>43042</v>
+      </c>
+      <c r="E14" s="19" t="s">
+        <v>16</v>
+      </c>
+      <c r="F14" t="s">
+        <v>16</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B1:E1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
+  <tableParts count="2">
+    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId3"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B36" sqref="B36"/>
+      <selection activeCell="B40" sqref="B40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3303,7 +4059,7 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
@@ -3380,7 +4136,7 @@
         <v>1</v>
       </c>
       <c r="B8" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
@@ -3427,265 +4183,307 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J16"/>
+  <dimension ref="A1:F31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C36" sqref="C36"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B36" sqref="B36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.42578125" customWidth="1"/>
-    <col min="2" max="2" width="26.140625" customWidth="1"/>
-    <col min="3" max="3" width="37.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.140625" customWidth="1"/>
-    <col min="5" max="5" width="37.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="34.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="30.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="35" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="22.5703125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.7109375" customWidth="1"/>
+    <col min="2" max="2" width="36.5703125" customWidth="1"/>
+    <col min="3" max="3" width="22" customWidth="1"/>
+    <col min="4" max="4" width="20.85546875" customWidth="1"/>
+    <col min="5" max="5" width="21.28515625" customWidth="1"/>
+    <col min="6" max="6" width="13.5703125" customWidth="1"/>
+    <col min="7" max="7" width="33.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="7" t="s">
-        <v>117</v>
-      </c>
-      <c r="B1" s="7"/>
-    </row>
-    <row r="2" spans="1:10" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" s="6" t="s">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="6" t="s">
         <v>92</v>
       </c>
-      <c r="B3" s="32" t="s">
-        <v>144</v>
-      </c>
-      <c r="C3" s="32"/>
-      <c r="D3" s="32"/>
-      <c r="E3" s="32"/>
-    </row>
-    <row r="5" spans="1:10" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B1" s="33" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="33"/>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="B5" s="19" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" s="19" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="C6" s="19" t="s">
-        <v>115</v>
-      </c>
-      <c r="D6" s="19" t="s">
-        <v>116</v>
-      </c>
-      <c r="E6" s="20" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B6" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>6</v>
+      </c>
+      <c r="C9" t="s">
+        <v>7</v>
+      </c>
+      <c r="D9" t="s">
+        <v>8</v>
+      </c>
+      <c r="E9" s="31" t="s">
         <v>9</v>
       </c>
-      <c r="F6" s="20" t="s">
-        <v>7</v>
-      </c>
-      <c r="G6" s="20" t="s">
-        <v>8</v>
-      </c>
-      <c r="H6" s="20" t="s">
+      <c r="F9" s="31" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B10" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C10">
+        <v>100</v>
+      </c>
+      <c r="D10">
+        <v>95</v>
+      </c>
+      <c r="E10" t="s">
+        <v>12</v>
+      </c>
+      <c r="F10" s="1">
+        <v>0.95</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B11" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C11">
+        <v>99</v>
+      </c>
+      <c r="D11">
+        <v>90</v>
+      </c>
+      <c r="E11" t="s">
+        <v>12</v>
+      </c>
+      <c r="F11" s="1">
+        <v>0.91</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B12" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C12">
+        <v>9.5</v>
+      </c>
+      <c r="D12">
+        <v>8.5</v>
+      </c>
+      <c r="E12" t="s">
+        <v>12</v>
+      </c>
+      <c r="F12" s="1">
+        <v>0.89</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B13" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C13">
+        <v>0</v>
+      </c>
+      <c r="D13">
+        <v>10</v>
+      </c>
+      <c r="E13" t="s">
+        <v>12</v>
+      </c>
+      <c r="F13" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B14" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C14">
+        <v>0</v>
+      </c>
+      <c r="D14">
+        <v>0</v>
+      </c>
+      <c r="E14" t="s">
+        <v>13</v>
+      </c>
+      <c r="F14" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="B17" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="3" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B21" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B22" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B25" t="s">
+        <v>6</v>
+      </c>
+      <c r="C25" t="s">
         <v>26</v>
       </c>
-      <c r="I6" s="20" t="s">
+      <c r="D25" t="s">
         <v>24</v>
       </c>
-      <c r="J6" s="20" t="s">
+      <c r="E25" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="7" spans="1:10" s="19" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="5">
-        <v>1</v>
-      </c>
-      <c r="C7" s="21">
-        <v>43024</v>
-      </c>
-      <c r="D7" s="22">
-        <v>43028</v>
-      </c>
-      <c r="E7" s="4" t="s">
+      <c r="F25" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B26" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C26" t="s">
         <v>12</v>
       </c>
-      <c r="F7" s="4">
-        <v>10</v>
-      </c>
-      <c r="G7" s="4">
-        <v>8</v>
-      </c>
-      <c r="H7" s="4" t="s">
+      <c r="D26">
+        <v>100</v>
+      </c>
+      <c r="E26">
+        <v>5</v>
+      </c>
+      <c r="F26" s="1">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B27" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C27" t="s">
         <v>12</v>
       </c>
-      <c r="I7" s="4">
+      <c r="D27">
+        <v>99</v>
+      </c>
+      <c r="E27">
+        <v>5.67</v>
+      </c>
+      <c r="F27" s="1">
+        <v>5.7000000000000002E-2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B28" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="C28" t="s">
+        <v>12</v>
+      </c>
+      <c r="D28">
         <v>100</v>
       </c>
-      <c r="J7" s="4">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" s="19" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="19">
-        <v>2</v>
-      </c>
-      <c r="C8" s="23">
-        <v>43031</v>
-      </c>
-      <c r="D8" s="24">
-        <v>43035</v>
-      </c>
-      <c r="E8" s="4" t="s">
+      <c r="E28">
+        <v>0</v>
+      </c>
+      <c r="F28" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B29" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C29" t="s">
         <v>13</v>
       </c>
-      <c r="F8" s="4">
+      <c r="D29">
         <v>0</v>
       </c>
-      <c r="G8" s="4">
+      <c r="E29">
         <v>0</v>
       </c>
-      <c r="H8" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="I8" s="4">
-        <v>35</v>
-      </c>
-      <c r="J8" s="4">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" s="19" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="19">
-        <v>3</v>
-      </c>
-      <c r="C9" s="21">
-        <v>43038</v>
-      </c>
-      <c r="D9" s="22">
-        <v>43042</v>
-      </c>
-      <c r="E9" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="F9" s="4">
-        <v>0</v>
-      </c>
-      <c r="G9" s="4">
-        <v>0</v>
-      </c>
-      <c r="H9" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="I9" s="4">
-        <v>0</v>
-      </c>
-      <c r="J9" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" s="19" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="11" spans="1:10" s="19" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B11" s="19" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" s="19" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B12" s="19" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" s="19" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="19" t="s">
-        <v>40</v>
-      </c>
-      <c r="C13" s="19" t="s">
-        <v>30</v>
-      </c>
-      <c r="D13" s="19" t="s">
-        <v>31</v>
-      </c>
-      <c r="E13" s="19" t="s">
-        <v>10</v>
-      </c>
-      <c r="F13" s="19" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" s="19" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="19">
-        <v>1</v>
-      </c>
-      <c r="C14" s="21">
-        <v>43024</v>
-      </c>
-      <c r="D14" s="22">
-        <v>43028</v>
-      </c>
-      <c r="E14" s="1">
-        <v>0.8</v>
-      </c>
-      <c r="F14" s="1">
-        <v>0.05</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" s="19" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="19">
-        <v>2</v>
-      </c>
-      <c r="C15" s="23">
-        <v>43031</v>
-      </c>
-      <c r="D15" s="24">
-        <v>43035</v>
-      </c>
-      <c r="E15" s="19" t="s">
+      <c r="F29" t="s">
         <v>16</v>
       </c>
-      <c r="F15" s="29">
-        <f>10/35</f>
-        <v>0.2857142857142857</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B16">
-        <v>3</v>
-      </c>
-      <c r="C16" s="21">
-        <v>43038</v>
-      </c>
-      <c r="D16" s="22">
-        <v>43042</v>
-      </c>
-      <c r="E16" s="19" t="s">
-        <v>16</v>
-      </c>
-      <c r="F16" t="s">
-        <v>16</v>
-      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A30" s="5"/>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E31" s="19"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="B3:E3"/>
+    <mergeCell ref="B1:C1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
   <tableParts count="2">
-    <tablePart r:id="rId2"/>
     <tablePart r:id="rId3"/>
+    <tablePart r:id="rId4"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>